<commit_message>
Updated the data objects and assertions for the Alabama, Illinois, and Dev environments
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29711"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C55BD339-A831-4EE5-BA73-421943FD0A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC2E5A4C-20DB-47BC-A41B-4B768E91DF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="procedure_April2025Change" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="79">
   <si>
     <t>Action</t>
   </si>
@@ -247,6 +247,24 @@
   </si>
   <si>
     <t>Car passenger injured in collision with pedestrian or animal in nontraffic accident, initial encounter</t>
+  </si>
+  <si>
+    <t>V60.0XXA</t>
+  </si>
+  <si>
+    <t>Driver of heavy transport vehicle injured in collision with pedestrian or animal in nontraffic accident, initial encounter</t>
+  </si>
+  <si>
+    <t>Y21.0XXA</t>
+  </si>
+  <si>
+    <t>Drowning and submersion while in bathtub, undetermined intent, initial encounter</t>
+  </si>
+  <si>
+    <t>T51.0X1A</t>
+  </si>
+  <si>
+    <t>Toxic effect of ethanol, accidental (unintentional), initial encounter</t>
   </si>
   <si>
     <t>T68.XXXA</t>
@@ -306,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -318,7 +336,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
@@ -637,7 +654,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1155,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE3D585-7D25-4CA2-94DE-DEE69EE26564}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1191,15 +1208,6 @@
       <c r="F1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="45.75">
       <c r="A2" s="1" t="s">
@@ -1220,7 +1228,6 @@
       <c r="F2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="5"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1246,7 +1253,6 @@
       <c r="F3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="5"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1272,7 +1278,6 @@
       <c r="F4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="5"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1298,7 +1303,6 @@
       <c r="F5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="5"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1324,7 +1328,6 @@
       <c r="F6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="5"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1332,13 +1335,6 @@
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1352,13 +1348,6 @@
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1371,195 +1360,6 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1569,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA336EA7-D253-4A5E-A32F-223F8B21749A}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1626,7 +1426,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45.75">
+    <row r="4" spans="1:5" ht="183">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1640,7 +1440,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="91.5">
+    <row r="5" spans="1:5" ht="121.5">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1648,24 +1448,24 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="137.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="91.5">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>69</v>
+      <c r="C6" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45.75">
@@ -1676,10 +1476,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>